<commit_message>
updated action item list from last call
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1060" yWindow="2920" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To-do list'!$B$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To-do list'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
-  <si>
-    <t>Done?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Notes</t>
   </si>
@@ -36,9 +33,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Project 3</t>
   </si>
   <si>
@@ -109,6 +103,18 @@
   </si>
   <si>
     <t>python prototype to add random data to a table you plumb'd</t>
+  </si>
+  <si>
+    <t>update git and clone repository on server</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Done?2</t>
+  </si>
+  <si>
+    <t>install latest version of python (activestate python)</t>
   </si>
 </sst>
 </file>
@@ -164,15 +170,21 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,8 +192,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -203,8 +226,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,8 +258,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -241,6 +273,9 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -251,9 +286,60 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -323,29 +409,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -478,13 +541,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="B2:E28" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="B2:E28"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Done?" dataDxfId="3"/>
-    <tableColumn id="2" name="Project 3" dataDxfId="2"/>
-    <tableColumn id="3" name="Due By" dataDxfId="1"/>
-    <tableColumn id="4" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A2:E30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A2:E30"/>
+  <sortState ref="A3:E30">
+    <sortCondition ref="A2:A30"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="5" name="Order" dataDxfId="1"/>
+    <tableColumn id="6" name="Done?2" dataDxfId="0"/>
+    <tableColumn id="2" name="Project 3" dataDxfId="4"/>
+    <tableColumn id="3" name="Due By" dataDxfId="3"/>
+    <tableColumn id="4" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -725,16 +792,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="70.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="36.83203125" style="1" customWidth="1"/>
@@ -746,6 +813,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
@@ -754,27 +822,37 @@
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>1</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5">
+        <v>40426</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
@@ -785,15 +863,17 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C4" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5">
         <v>40426</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -802,170 +882,185 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5">
         <v>40426</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1">
       <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5">
-        <v>40426</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" customHeight="1">
       <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>3.1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="D7" s="5">
+        <v>40651</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5">
-        <v>40286</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="A9" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="1">
         <v>4</v>
       </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5">
-        <v>40651</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" customHeight="1">
       <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" customHeight="1">
       <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A14" s="1">
-        <v>6</v>
-      </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5">
+        <v>40286</v>
+      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" customHeight="1">
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" customHeight="1">
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" customHeight="1">
+    <row r="17" spans="2:7" ht="16.5" customHeight="1">
       <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" customHeight="1">
+    <row r="18" spans="2:7" ht="16.5" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -973,105 +1068,110 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1">
+    <row r="19" spans="2:7" ht="16.5" customHeight="1">
       <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B20" s="2"/>
-      <c r="C20" s="4" t="s">
-        <v>21</v>
-      </c>
+    <row r="20" spans="2:7" ht="16.5" customHeight="1">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B21" s="2"/>
+    <row r="21" spans="2:7" ht="16.5" customHeight="1">
+      <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
+    <row r="22" spans="2:7" ht="16.5" customHeight="1">
+      <c r="B22" s="3"/>
+      <c r="C22" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="2"/>
+    <row r="23" spans="2:7">
+      <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="E23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7">
-      <c r="B24" s="2"/>
+    <row r="24" spans="2:7">
+      <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="2:7">
       <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="2:7">
       <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="2:7">
       <c r="B27" s="3"/>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1">
-        <v>5</v>
-      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="2:7">
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D23:D28 D3:D20">
+  <conditionalFormatting sqref="D23:D30 D3:D20">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1081,7 +1181,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B30">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
completed a few more AIs, added a few new ones as well
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="2920" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Notes</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>install latest version of python (activestate python)</t>
+  </si>
+  <si>
+    <t>upload latest stock predictions</t>
   </si>
 </sst>
 </file>
@@ -233,12 +236,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -311,54 +311,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor indexed="9"/>
         </patternFill>
       </fill>
@@ -409,6 +361,54 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -547,11 +547,11 @@
     <sortCondition ref="A2:A30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" name="Order" dataDxfId="1"/>
-    <tableColumn id="6" name="Done?2" dataDxfId="0"/>
-    <tableColumn id="2" name="Project 3" dataDxfId="4"/>
-    <tableColumn id="3" name="Due By" dataDxfId="3"/>
-    <tableColumn id="4" name="Notes" dataDxfId="2"/>
+    <tableColumn id="5" name="Order" dataDxfId="4"/>
+    <tableColumn id="6" name="Done?2" dataDxfId="3"/>
+    <tableColumn id="2" name="Project 3" dataDxfId="2"/>
+    <tableColumn id="3" name="Due By" dataDxfId="1"/>
+    <tableColumn id="4" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -795,7 +795,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -813,361 +813,370 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>40426</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>40426</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>40426</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" customHeight="1">
       <c r="A7" s="1">
         <v>3.1</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>40651</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1">
       <c r="A8" s="1">
         <v>3.2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" customHeight="1">
       <c r="A9" s="1">
         <v>3.3</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1">
       <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" customHeight="1">
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" customHeight="1">
       <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B14" s="3"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>40286</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B17" s="3"/>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="3"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4" t="s">
+      <c r="D25" s="4"/>
+      <c r="E25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="3"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
adding cloudfoundry as part of architecture research
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Notes</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>upload latest stock predictions</t>
+  </si>
+  <si>
+    <t>see how cloud foundry can be used for stocrates (http://blog.cloudfoundry.com/)</t>
   </si>
 </sst>
 </file>
@@ -795,7 +798,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1174,9 +1177,13 @@
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
need to modify schema to add industry
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="620" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="6520" yWindow="460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Notes</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>modifying the schema to add industry per stock</t>
   </si>
 </sst>
 </file>
@@ -854,7 +857,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1345,9 +1348,13 @@
     <row r="39" spans="1:6">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6">

</xml_diff>

<commit_message>
updated action items as of 5/2 meeting
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="460" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="8300" yWindow="1860" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Notes</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Project 3</t>
   </si>
   <si>
-    <t>python backend</t>
-  </si>
-  <si>
     <t>php front-end data entry</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>python email prototype, password entry through a config file. .stocrates</t>
   </si>
   <si>
-    <t>python data insertion into DB</t>
-  </si>
-  <si>
     <t>python2 (separate script) every night run to check against prediction</t>
   </si>
   <si>
@@ -84,27 +78,15 @@
     <t>python2 run algorithm to gauge analyst accuracy index. (0-100)</t>
   </si>
   <si>
-    <t>create accuracy index algorithim (ACCIA)</t>
-  </si>
-  <si>
     <t>python needs to extract stock's KPIs (market cap, current price etc)</t>
   </si>
   <si>
     <t>figure out stock KPIs</t>
   </si>
   <si>
-    <t>OA/DB whiteboard this</t>
-  </si>
-  <si>
-    <t>python need to do some extrapolation calculations as well</t>
-  </si>
-  <si>
     <t>php myadmin explore (db admin for mysql)</t>
   </si>
   <si>
-    <t>python prototype to add random data to a table you plumb'd</t>
-  </si>
-  <si>
     <t>update git and clone repository on server</t>
   </si>
   <si>
@@ -126,9 +108,6 @@
     <t xml:space="preserve">mysql db library </t>
   </si>
   <si>
-    <t>active state 2.7 install</t>
-  </si>
-  <si>
     <t>update schema to link to image within email</t>
   </si>
   <si>
@@ -153,7 +132,37 @@
     <t>modifying the schema to add industry per stock</t>
   </si>
   <si>
-    <t>review cisco conflict of interest policy and and new business request</t>
+    <t>create stAR (stocrates Analyst Ranker) algorithm</t>
+  </si>
+  <si>
+    <t>python data insertion into DB via script</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>fix imaplib</t>
+  </si>
+  <si>
+    <t>make python email prototype work on imac</t>
+  </si>
+  <si>
+    <t>push dummy data through phpMyAdmin</t>
+  </si>
+  <si>
+    <t>document stAR algorithm thus far</t>
+  </si>
+  <si>
+    <t>document HLA thus far</t>
+  </si>
+  <si>
+    <t>finance.yahoo API (simple csv method not using YahooQL)</t>
+  </si>
+  <si>
+    <t>investigate open source license</t>
+  </si>
+  <si>
+    <t>Omer : set up eclipse to write code</t>
   </si>
 </sst>
 </file>
@@ -163,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -173,12 +182,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -250,36 +253,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,27 +294,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -323,6 +325,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +339,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -605,10 +609,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A2:F40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A2:F40"/>
-  <sortState ref="A3:E30">
-    <sortCondition ref="A2:A30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A2:F35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A2:F35"/>
+  <sortState ref="A3:F35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="5" name="Order" dataDxfId="5"/>
@@ -857,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -887,11 +891,11 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>28</v>
+      <c r="A2" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -903,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -915,13 +919,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
         <v>40426</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -933,14 +937,14 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="4">
         <v>40426</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -953,13 +957,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4">
         <v>40426</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -970,11 +974,11 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -987,192 +991,237 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4">
         <v>40651</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1">
       <c r="A8" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" customHeight="1">
       <c r="A9" s="1">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1">
       <c r="A10" s="1">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>3.3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" customHeight="1">
       <c r="A11" s="1">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="10" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A12" s="1">
-        <v>6</v>
+      <c r="A12" s="2">
+        <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A13" s="1">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="10"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B14" s="2"/>
-      <c r="C14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4">
-        <v>40286</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A16" s="1">
+        <v>5.5</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A17" s="1">
+        <v>6</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1">
       <c r="A18" s="1">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A20" s="2">
+        <v>9</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
@@ -1180,202 +1229,198 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A22" s="2">
+        <v>10.1</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="10"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A23" s="1">
+        <v>11</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>11.1</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="11"/>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="10"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7">
+      <c r="A25" s="2">
+        <v>11.2</v>
+      </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="F25" s="10"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7">
+      <c r="A26" s="2">
+        <v>11.3</v>
+      </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:7">
+      <c r="A27" s="2">
+        <v>12</v>
+      </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:7">
+      <c r="A28" s="2">
+        <v>13</v>
+      </c>
       <c r="B28" s="2"/>
       <c r="C28" s="3" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>14</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="11"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>15</v>
+      </c>
       <c r="B30" s="2"/>
       <c r="C30" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="11"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1">
+        <v>16</v>
+      </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1">
+        <v>90</v>
+      </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="11"/>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1">
+        <v>99</v>
+      </c>
       <c r="B33" s="2"/>
       <c r="C33" s="3" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2">
+        <v>99.1</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="11"/>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" ht="30">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="F35" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D23:D40 D3:D20">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="D24:D35 D3:D21">
+    <cfRule type="iconSet" priority="6">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="TODAY()-7"/>
@@ -1384,7 +1429,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B35">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
new action list for solo work
</commit_message>
<xml_diff>
--- a/etc/stocrates-AI-List.xlsx
+++ b/etc/stocrates-AI-List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>Notes</t>
   </si>
@@ -117,9 +117,6 @@
     <t>OA/DB</t>
   </si>
   <si>
-    <t>work on front-end which lets you query a Stock and provide recommendations based on analyst feedback with respective confidence rating</t>
-  </si>
-  <si>
     <t>install mysqlDB extension (provided by daniel)</t>
   </si>
   <si>
@@ -222,7 +219,43 @@
     <t>data: barrons new newspapers, take pictures, write rec text and send to gmail</t>
   </si>
   <si>
-    <t xml:space="preserve">coding: </t>
+    <t>mongoDB: create the .js file which creates the schema</t>
+  </si>
+  <si>
+    <t>mongoDB: create the .sj file which creates input DUMMY data</t>
+  </si>
+  <si>
+    <t>coding: write code to extract data from gmail and insert into database</t>
+  </si>
+  <si>
+    <t>coding: research finance.yahoo API and decorate the stock with data (simple csv method not using YahooQL)</t>
+  </si>
+  <si>
+    <t>coding: write code to make a daemon which runs in the background and issues commands at certain times, or with certain input</t>
+  </si>
+  <si>
+    <t>coding: use daemon code to pull data from gmail</t>
+  </si>
+  <si>
+    <t>coding: write stAR to populate rating fields based on logic</t>
+  </si>
+  <si>
+    <t>coding: create a flow chart for stAR logic</t>
+  </si>
+  <si>
+    <t>coding: insertion create option to insert text data via website</t>
+  </si>
+  <si>
+    <t>coding: view work on front-end which lets you query a Stock and provide recommendations based on analyst feedback with respective confidence rating</t>
+  </si>
+  <si>
+    <t>coding: insertion create option to drag and drop an image of a recommendation (gmail style)</t>
+  </si>
+  <si>
+    <t>coding: investigate open source licensing</t>
+  </si>
+  <si>
+    <t>coding:  run algorithm to gauge analyst accuracy index. (0-100)</t>
   </si>
 </sst>
 </file>
@@ -313,8 +346,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -379,7 +426,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -398,6 +445,13 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -416,6 +470,13 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -685,8 +746,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A2:F70" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A2:F70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A2:F72" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A2:F72">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A3:F35">
     <sortCondition ref="A2:A35"/>
   </sortState>
@@ -937,10 +1002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -983,11 +1049,11 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" customHeight="1">
+    <row r="3" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1006,7 +1072,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1">
+    <row r="4" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1025,7 +1091,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" customHeight="1">
+    <row r="5" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1044,13 +1110,15 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" customHeight="1">
+    <row r="6" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
@@ -1059,7 +1127,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A7" s="1">
         <v>3.1</v>
       </c>
@@ -1078,20 +1146,22 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" customHeight="1">
+    <row r="8" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A8" s="1">
         <v>3.1</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" customHeight="1">
+    <row r="9" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A9" s="1">
         <v>3.2</v>
       </c>
@@ -1108,7 +1178,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" customHeight="1">
+    <row r="10" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A10" s="1">
         <v>3.3</v>
       </c>
@@ -1125,7 +1195,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" customHeight="1">
+    <row r="11" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1142,24 +1212,26 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" customHeight="1">
+    <row r="12" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A12" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" customHeight="1">
+    <row r="13" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A13" s="2">
         <v>4.2</v>
       </c>
@@ -1176,7 +1248,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" customHeight="1">
+    <row r="14" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A14" s="2">
         <v>4.3</v>
       </c>
@@ -1184,18 +1256,18 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" customHeight="1">
+    <row r="15" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1212,11 +1284,13 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" customHeight="1">
+    <row r="16" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A16" s="1">
         <v>5.5</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1227,11 +1301,13 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" customHeight="1">
+    <row r="17" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A17" s="1">
         <v>6</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1242,11 +1318,13 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" customHeight="1">
+    <row r="18" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A18" s="1">
         <v>7</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1257,45 +1335,51 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1">
+    <row r="19" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1">
+    <row r="20" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A20" s="2">
         <v>9</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" customHeight="1">
+    <row r="21" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A21" s="1">
         <v>10</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1304,13 +1388,15 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" customHeight="1">
+    <row r="22" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A22" s="2">
         <v>10.1</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="3" t="s">
@@ -1319,28 +1405,32 @@
       <c r="F22" s="10"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" customHeight="1">
+    <row r="23" spans="1:7" ht="16.5" hidden="1" customHeight="1">
       <c r="A23" s="1">
         <v>11</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="1">
         <v>11.1</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
@@ -1349,11 +1439,13 @@
       <c r="F24" s="10"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="2">
         <v>11.2</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1364,25 +1456,29 @@
       <c r="F25" s="10"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="2">
         <v>11.3</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="2">
         <v>12</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="3" t="s">
@@ -1390,13 +1486,15 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="2">
         <v>13</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="3" t="s">
@@ -1404,11 +1502,13 @@
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="1">
         <v>14</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
@@ -1416,11 +1516,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="1">
         <v>15</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C30" s="3" t="s">
         <v>17</v>
       </c>
@@ -1428,11 +1530,13 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="1">
         <v>16</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>16</v>
       </c>
@@ -1440,11 +1544,13 @@
       <c r="E31" s="3"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="1">
         <v>90</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
@@ -1454,11 +1560,13 @@
       </c>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33" s="1">
         <v>99</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1468,35 +1576,33 @@
       </c>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" ht="30">
-      <c r="A34" s="2">
-        <v>99.1</v>
-      </c>
-      <c r="B34" s="2"/>
+    <row r="34" spans="1:6" hidden="1">
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C34" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6">
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E35" s="3"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D36" s="4"/>
       <c r="E36" s="3"/>
       <c r="F36" s="10"/>
@@ -1555,7 +1661,7 @@
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
@@ -1565,7 +1671,7 @@
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="3"/>
@@ -1575,7 +1681,7 @@
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="3"/>
@@ -1584,9 +1690,7 @@
     <row r="45" spans="1:6">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="4"/>
       <c r="E45" s="3"/>
       <c r="F45" s="10"/>
@@ -1594,7 +1698,9 @@
     <row r="46" spans="1:6">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="D46" s="4"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
@@ -1602,7 +1708,9 @@
     <row r="47" spans="1:6">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D47" s="4"/>
       <c r="E47" s="3"/>
       <c r="F47" s="10"/>
@@ -1611,7 +1719,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="3"/>
@@ -1621,7 +1729,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="3"/>
@@ -1640,7 +1748,9 @@
     <row r="51" spans="1:6">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D51" s="4"/>
       <c r="E51" s="3"/>
       <c r="F51" s="10"/>
@@ -1649,7 +1759,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="3"/>
@@ -1659,7 +1769,7 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="3"/>
@@ -1668,9 +1778,7 @@
     <row r="54" spans="1:6">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="C54" s="3"/>
       <c r="D54" s="4"/>
       <c r="E54" s="3"/>
       <c r="F54" s="10"/>
@@ -1688,7 +1796,9 @@
     <row r="56" spans="1:6">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
-      <c r="C56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D56" s="4"/>
       <c r="E56" s="3"/>
       <c r="F56" s="10"/>
@@ -1697,7 +1807,7 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
@@ -1706,9 +1816,7 @@
     <row r="58" spans="1:6">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="C58" s="3"/>
       <c r="D58" s="4"/>
       <c r="E58" s="3"/>
       <c r="F58" s="10"/>
@@ -1717,7 +1825,7 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="3"/>
@@ -1735,25 +1843,27 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="3"/>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" ht="30">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D62" s="4"/>
       <c r="E62" s="3"/>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" ht="30">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="3"/>
@@ -1762,7 +1872,9 @@
     <row r="64" spans="1:6">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="D64" s="4"/>
       <c r="E64" s="3"/>
       <c r="F64" s="10"/>
@@ -1770,7 +1882,9 @@
     <row r="65" spans="1:6">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D65" s="4"/>
       <c r="E65" s="3"/>
       <c r="F65" s="10"/>
@@ -1778,7 +1892,9 @@
     <row r="66" spans="1:6">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D66" s="4"/>
       <c r="E66" s="3"/>
       <c r="F66" s="10"/>
@@ -1786,15 +1902,19 @@
     <row r="67" spans="1:6">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="D67" s="4"/>
       <c r="E67" s="3"/>
       <c r="F67" s="10"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" ht="30">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="D68" s="4"/>
       <c r="E68" s="3"/>
       <c r="F68" s="10"/>
@@ -1802,23 +1922,45 @@
     <row r="69" spans="1:6">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
-      <c r="C69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D69" s="4"/>
       <c r="E69" s="3"/>
       <c r="F69" s="10"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" ht="30">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="3"/>
+      <c r="C70" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D70" s="4"/>
       <c r="E70" s="3"/>
       <c r="F70" s="10"/>
     </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D24:D70 D3:D21">
-    <cfRule type="iconSet" priority="6">
+  <conditionalFormatting sqref="D24:D72 D3:D21">
+    <cfRule type="iconSet" priority="8">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="TODAY()-7"/>
@@ -1827,7 +1969,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B72">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>